<commit_message>
Review document and update minor items #84
</commit_message>
<xml_diff>
--- a/Documentation/src/03_project-documentation/project_plan.xlsx
+++ b/Documentation/src/03_project-documentation/project_plan.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\bnz\dev-workspace\kubewatch\Documentation\src\03_project-documentation\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{A82A63B5-8FFC-4F23-8739-27585C9BD4CB}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{3A41A904-D783-4544-94E3-2264ED46F9CE}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-103" yWindow="-103" windowWidth="23657" windowHeight="15394" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15990" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -30,7 +30,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="90" uniqueCount="89">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="89" uniqueCount="89">
   <si>
     <t>Project Planning - KubeWatch</t>
   </si>
@@ -155,9 +155,6 @@
     <t>Rough Project Plan (RUD)</t>
   </si>
   <si>
-    <t>Detailled Porject Plan (Scrum)</t>
-  </si>
-  <si>
     <t>Meeting Plan</t>
   </si>
   <si>
@@ -182,81 +179,39 @@
     <t>Kubernetes Cluster</t>
   </si>
   <si>
-    <t>Website</t>
-  </si>
-  <si>
     <t>Implementation</t>
   </si>
   <si>
     <t>Milestones:</t>
   </si>
   <si>
-    <t>K8's Cluster (Local)</t>
-  </si>
-  <si>
     <t>M1: Project Plan</t>
   </si>
   <si>
-    <t>K8's Cluster (Server)</t>
-  </si>
-  <si>
     <t>M2: Requirements</t>
   </si>
   <si>
-    <t>K8's Cluster (GitLab)</t>
-  </si>
-  <si>
     <t>M3: End of Elaboration &amp; Arch. Prototype</t>
   </si>
   <si>
-    <t>K8's Cluster (Functionality)</t>
-  </si>
-  <si>
     <t>M4: Quality</t>
   </si>
   <si>
-    <t>Website (GitLab)</t>
-  </si>
-  <si>
     <t>M5: Architecture</t>
   </si>
   <si>
-    <t>Website (Functionality)</t>
-  </si>
-  <si>
     <t>M6: Project Presentation</t>
   </si>
   <si>
     <t>Test</t>
   </si>
   <si>
-    <t>K8's Local Cluster Implementation</t>
-  </si>
-  <si>
-    <t>K8's Server Cluster Implementation</t>
-  </si>
-  <si>
-    <t>K8's GitLab Implementation</t>
-  </si>
-  <si>
-    <t>K8's Cluster Functionality</t>
-  </si>
-  <si>
-    <t>Website GitLab Implementation</t>
-  </si>
-  <si>
-    <t>Website Functionality</t>
-  </si>
-  <si>
     <t>Integration Test</t>
   </si>
   <si>
     <t>Deployment</t>
   </si>
   <si>
-    <t>K8's Cluster and Website combination</t>
-  </si>
-  <si>
     <t>Configuration &amp; Change Management</t>
   </si>
   <si>
@@ -297,6 +252,51 @@
   </si>
   <si>
     <t>Continuous improvement</t>
+  </si>
+  <si>
+    <t>Dashboard</t>
+  </si>
+  <si>
+    <t>Dashboard (GitLab)</t>
+  </si>
+  <si>
+    <t>Dashboard (Functionality)</t>
+  </si>
+  <si>
+    <t>Dashboard GitLab Implementation</t>
+  </si>
+  <si>
+    <t>Dashboard Functionality</t>
+  </si>
+  <si>
+    <t>Detailed Project Plan (Scrum)</t>
+  </si>
+  <si>
+    <t>K8s Cluster (Local)</t>
+  </si>
+  <si>
+    <t>K8s Cluster (Server)</t>
+  </si>
+  <si>
+    <t>K8s Cluster (GitLab)</t>
+  </si>
+  <si>
+    <t>K8s Cluster (Functionality)</t>
+  </si>
+  <si>
+    <t>K8s Local Cluster Implementation</t>
+  </si>
+  <si>
+    <t>K8s Server Cluster Implementation</t>
+  </si>
+  <si>
+    <t>K8s GitLab Implementation</t>
+  </si>
+  <si>
+    <t>K8s Cluster Functionality</t>
+  </si>
+  <si>
+    <t>K8s Cluster and Website combination</t>
   </si>
 </sst>
 </file>
@@ -304,13 +304,20 @@
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
   <numFmts count="1">
-    <numFmt numFmtId="165" formatCode="dd/mm"/>
+    <numFmt numFmtId="164" formatCode="dd/mm"/>
   </numFmts>
-  <fonts count="5" x14ac:knownFonts="1">
+  <fonts count="6" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
       <name val="Calibri"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color theme="1"/>
+      <name val="Calibri"/>
+      <family val="2"/>
       <scheme val="minor"/>
     </font>
     <font>
@@ -1027,11 +1034,11 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="168">
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+  <cellXfs count="170">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="0" fillId="6" borderId="0" xfId="0" applyFill="1"/>
     <xf numFmtId="0" fontId="0" fillId="7" borderId="0" xfId="0" applyFill="1"/>
     <xf numFmtId="0" fontId="0" fillId="4" borderId="0" xfId="0" applyFill="1" applyBorder="1"/>
@@ -1061,24 +1068,11 @@
     <xf numFmtId="0" fontId="0" fillId="4" borderId="4" xfId="0" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="4" borderId="5" xfId="0" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="6" borderId="8" xfId="0" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="17" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="6" borderId="17" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
-      <alignment horizontal="left"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="3" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
-      <alignment horizontal="left"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="4" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
-      <alignment horizontal="left"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="5" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="19" xfId="0" applyBorder="1" applyAlignment="1">
@@ -1096,7 +1090,6 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="25" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="26" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="6" borderId="25" xfId="0" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="8" borderId="27" xfId="0" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="8" borderId="28" xfId="0" applyFill="1" applyBorder="1"/>
@@ -1136,7 +1129,7 @@
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="27" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="6" borderId="26" xfId="0" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="26" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="26" xfId="0" applyFont="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="9" borderId="25" xfId="0" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="9" borderId="27" xfId="0" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="9" borderId="28" xfId="0" applyFill="1" applyBorder="1"/>
@@ -1146,7 +1139,7 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="27" xfId="0" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="29" xfId="0" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="9" borderId="30" xfId="0" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="32" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="32" xfId="0" applyFont="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="9" borderId="31" xfId="0" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="9" borderId="39" xfId="0" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="9" borderId="40" xfId="0" applyFill="1" applyBorder="1"/>
@@ -1162,10 +1155,10 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="40" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="41" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="42" xfId="0" applyBorder="1"/>
-    <xf numFmtId="0" fontId="3" fillId="11" borderId="18" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="4" fillId="11" borderId="18" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
-    <xf numFmtId="0" fontId="3" fillId="11" borderId="44" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="4" fillId="11" borderId="44" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="6" borderId="19" xfId="0" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="6" borderId="22" xfId="0" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="6" borderId="23" xfId="0" applyFill="1" applyBorder="1"/>
@@ -1177,17 +1170,53 @@
     <xf numFmtId="0" fontId="0" fillId="6" borderId="19" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="6" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="2" fillId="6" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="6" borderId="20" xfId="0" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="6" borderId="34" xfId="0" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="8" borderId="33" xfId="0" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="20" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="20" xfId="0" applyFont="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="9" borderId="19" xfId="0" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="9" borderId="21" xfId="0" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="9" borderId="22" xfId="0" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="9" borderId="23" xfId="0" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="10" borderId="21" xfId="0" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="24" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="164" fontId="5" fillId="2" borderId="17" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="164" fontId="5" fillId="3" borderId="5" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="164" fontId="5" fillId="4" borderId="4" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="164" fontId="5" fillId="4" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="164" fontId="5" fillId="4" borderId="5" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="5" borderId="3" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="5" borderId="5" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="164" fontId="5" fillId="5" borderId="47" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="6" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="9" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="164" fontId="5" fillId="3" borderId="12" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="7" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="10" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="164" fontId="5" fillId="3" borderId="13" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="4" borderId="7" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="4" borderId="10" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="164" fontId="5" fillId="4" borderId="13" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="5" borderId="6" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="5" borderId="9" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="164" fontId="5" fillId="5" borderId="12" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="4" fillId="11" borderId="46" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="6" borderId="18" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="13" borderId="22" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="13" borderId="28" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="13" borderId="40" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="13" borderId="36" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="13" borderId="10" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="12" borderId="45" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="12" borderId="44" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="12" borderId="46" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
     <xf numFmtId="0" fontId="0" fillId="11" borderId="45" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
@@ -1197,51 +1226,31 @@
     <xf numFmtId="0" fontId="0" fillId="11" borderId="46" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="12" borderId="45" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="12" borderId="44" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="12" borderId="46" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="165" fontId="4" fillId="2" borderId="17" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="165" fontId="4" fillId="3" borderId="5" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="165" fontId="4" fillId="4" borderId="4" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="165" fontId="4" fillId="4" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="165" fontId="4" fillId="4" borderId="5" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="5" borderId="3" xfId="0" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="5" borderId="5" xfId="0" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="165" fontId="4" fillId="5" borderId="47" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="3" borderId="6" xfId="0" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="3" borderId="9" xfId="0" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="165" fontId="4" fillId="3" borderId="12" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="3" borderId="7" xfId="0" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="3" borderId="10" xfId="0" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="165" fontId="4" fillId="3" borderId="13" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="4" borderId="7" xfId="0" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="4" borderId="10" xfId="0" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="165" fontId="4" fillId="4" borderId="13" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="5" borderId="6" xfId="0" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="5" borderId="9" xfId="0" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="165" fontId="4" fillId="5" borderId="12" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="3" fillId="11" borderId="46" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="6" borderId="18" xfId="0" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="13" borderId="22" xfId="0" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="13" borderId="28" xfId="0" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="13" borderId="40" xfId="0" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="13" borderId="36" xfId="0" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="13" borderId="10" xfId="0" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="4" fillId="13" borderId="48" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
-    <xf numFmtId="0" fontId="4" fillId="13" borderId="26" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
-    <xf numFmtId="0" fontId="4" fillId="13" borderId="30" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="0" fillId="4" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
+    <xf numFmtId="0" fontId="0" fillId="5" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="13" borderId="48" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="13" borderId="26" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="13" borderId="30" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="26" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="34" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="20" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -1257,6 +1266,136 @@
     </ext>
   </extLst>
 </styleSheet>
+</file>
+
+<file path=xl/drawings/drawing1.xml><?xml version="1.0" encoding="utf-8"?>
+<xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>19</xdr:col>
+      <xdr:colOff>276225</xdr:colOff>
+      <xdr:row>0</xdr:row>
+      <xdr:rowOff>152401</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>21</xdr:col>
+      <xdr:colOff>114300</xdr:colOff>
+      <xdr:row>11</xdr:row>
+      <xdr:rowOff>142875</xdr:rowOff>
+    </xdr:to>
+    <xdr:sp macro="" textlink="">
+      <xdr:nvSpPr>
+        <xdr:cNvPr id="2" name="Rectangle 1">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{786B8EB3-F09A-408B-AD14-C9ABEAFADBD0}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvSpPr/>
+      </xdr:nvSpPr>
+      <xdr:spPr>
+        <a:xfrm>
+          <a:off x="9925050" y="152401"/>
+          <a:ext cx="2981325" cy="2285999"/>
+        </a:xfrm>
+        <a:prstGeom prst="rect">
+          <a:avLst/>
+        </a:prstGeom>
+      </xdr:spPr>
+      <xdr:style>
+        <a:lnRef idx="2">
+          <a:schemeClr val="accent1">
+            <a:shade val="50000"/>
+          </a:schemeClr>
+        </a:lnRef>
+        <a:fillRef idx="1">
+          <a:schemeClr val="accent1"/>
+        </a:fillRef>
+        <a:effectRef idx="0">
+          <a:schemeClr val="accent1"/>
+        </a:effectRef>
+        <a:fontRef idx="minor">
+          <a:schemeClr val="lt1"/>
+        </a:fontRef>
+      </xdr:style>
+      <xdr:txBody>
+        <a:bodyPr vertOverflow="clip" horzOverflow="clip" rtlCol="0" anchor="t"/>
+        <a:lstStyle/>
+        <a:p>
+          <a:pPr algn="l"/>
+          <a:r>
+            <a:rPr lang="en-GB" sz="1100"/>
+            <a:t>Instructions</a:t>
+          </a:r>
+          <a:r>
+            <a:rPr lang="en-GB" sz="1100" baseline="0"/>
+            <a:t> for producing a PNG:</a:t>
+          </a:r>
+        </a:p>
+        <a:p>
+          <a:pPr algn="l"/>
+          <a:endParaRPr lang="en-GB" sz="1100" baseline="0"/>
+        </a:p>
+        <a:p>
+          <a:pPr algn="l"/>
+          <a:r>
+            <a:rPr lang="en-GB" sz="1100" b="1" baseline="0"/>
+            <a:t>Windows</a:t>
+          </a:r>
+        </a:p>
+        <a:p>
+          <a:pPr algn="l"/>
+          <a:r>
+            <a:rPr lang="en-GB" sz="1100" baseline="0"/>
+            <a:t>1. Highlight all relevant cells (A1:R56)</a:t>
+          </a:r>
+        </a:p>
+        <a:p>
+          <a:pPr algn="l"/>
+          <a:r>
+            <a:rPr lang="en-GB" sz="1100" baseline="0"/>
+            <a:t>2. Open Paint :)</a:t>
+          </a:r>
+        </a:p>
+        <a:p>
+          <a:pPr algn="l"/>
+          <a:r>
+            <a:rPr lang="en-GB" sz="1100" baseline="0"/>
+            <a:t>3. Paste content</a:t>
+          </a:r>
+        </a:p>
+        <a:p>
+          <a:pPr algn="l"/>
+          <a:r>
+            <a:rPr lang="en-GB" sz="1100" baseline="0"/>
+            <a:t>4. Save as png</a:t>
+          </a:r>
+        </a:p>
+        <a:p>
+          <a:pPr algn="l"/>
+          <a:endParaRPr lang="en-GB" sz="1100" baseline="0"/>
+        </a:p>
+        <a:p>
+          <a:pPr algn="l"/>
+          <a:r>
+            <a:rPr lang="en-GB" sz="1100" b="1" baseline="0"/>
+            <a:t>Linux </a:t>
+          </a:r>
+        </a:p>
+        <a:p>
+          <a:pPr algn="l"/>
+          <a:r>
+            <a:rPr lang="en-GB" sz="1100" baseline="0"/>
+            <a:t>tbd</a:t>
+          </a:r>
+          <a:endParaRPr lang="en-CH" sz="1100"/>
+        </a:p>
+      </xdr:txBody>
+    </xdr:sp>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+</xdr:wsDr>
 </file>
 
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
@@ -1473,40 +1612,40 @@
   <sheetViews>
     <sheetView showGridLines="0" tabSelected="1" zoomScaleNormal="100" workbookViewId="0"/>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.6" x14ac:dyDescent="0.4"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="3.69140625" customWidth="1"/>
-    <col min="2" max="2" width="3.69140625" style="2" customWidth="1"/>
-    <col min="3" max="3" width="35.3046875" bestFit="1" customWidth="1"/>
-    <col min="4" max="18" width="6.3828125" bestFit="1" customWidth="1"/>
-    <col min="19" max="19" width="5.53515625" customWidth="1"/>
+    <col min="1" max="1" width="3.7109375" customWidth="1"/>
+    <col min="2" max="2" width="3.7109375" style="2" customWidth="1"/>
+    <col min="3" max="3" width="35.28515625" bestFit="1" customWidth="1"/>
+    <col min="4" max="18" width="6.42578125" bestFit="1" customWidth="1"/>
+    <col min="19" max="19" width="5.5703125" customWidth="1"/>
     <col min="20" max="20" width="38" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:18" ht="26.15" x14ac:dyDescent="0.7">
+    <row r="1" spans="1:18" ht="26.25" x14ac:dyDescent="0.4">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
       <c r="B1" s="1"/>
     </row>
-    <row r="2" spans="1:18" ht="15" thickBot="1" x14ac:dyDescent="0.45">
+    <row r="2" spans="1:18" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A2" s="2"/>
     </row>
-    <row r="3" spans="1:18" x14ac:dyDescent="0.4">
+    <row r="3" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A3" s="2"/>
       <c r="D3" s="19" t="s">
         <v>1</v>
       </c>
-      <c r="E3" s="146" t="s">
+      <c r="E3" s="134" t="s">
         <v>2</v>
       </c>
-      <c r="F3" s="149" t="s">
+      <c r="F3" s="137" t="s">
         <v>3</v>
       </c>
-      <c r="G3" s="149" t="s">
+      <c r="G3" s="137" t="s">
         <v>4</v>
       </c>
-      <c r="H3" s="149" t="s">
+      <c r="H3" s="137" t="s">
         <v>5</v>
       </c>
       <c r="I3" s="24" t="s">
@@ -1515,45 +1654,45 @@
       <c r="J3" s="27" t="s">
         <v>7</v>
       </c>
-      <c r="K3" s="152" t="s">
+      <c r="K3" s="140" t="s">
         <v>8</v>
       </c>
       <c r="L3" s="28" t="s">
         <v>9</v>
       </c>
-      <c r="M3" s="152" t="s">
+      <c r="M3" s="140" t="s">
         <v>10</v>
       </c>
       <c r="N3" s="28" t="s">
         <v>11</v>
       </c>
-      <c r="O3" s="152" t="s">
+      <c r="O3" s="140" t="s">
         <v>12</v>
       </c>
       <c r="P3" s="29" t="s">
         <v>13</v>
       </c>
-      <c r="Q3" s="155" t="s">
+      <c r="Q3" s="143" t="s">
         <v>14</v>
       </c>
-      <c r="R3" s="143" t="s">
+      <c r="R3" s="131" t="s">
         <v>15</v>
       </c>
     </row>
-    <row r="4" spans="1:18" x14ac:dyDescent="0.4">
+    <row r="4" spans="1:18" x14ac:dyDescent="0.25">
       <c r="D4" s="20" t="s">
         <v>17</v>
       </c>
-      <c r="E4" s="147" t="s">
+      <c r="E4" s="135" t="s">
         <v>18</v>
       </c>
-      <c r="F4" s="150" t="s">
+      <c r="F4" s="138" t="s">
         <v>19</v>
       </c>
-      <c r="G4" s="150" t="s">
+      <c r="G4" s="138" t="s">
         <v>20</v>
       </c>
-      <c r="H4" s="150" t="s">
+      <c r="H4" s="138" t="s">
         <v>21</v>
       </c>
       <c r="I4" s="25" t="s">
@@ -1562,94 +1701,94 @@
       <c r="J4" s="30" t="s">
         <v>23</v>
       </c>
-      <c r="K4" s="153"/>
+      <c r="K4" s="141"/>
       <c r="L4" s="6" t="s">
         <v>24</v>
       </c>
-      <c r="M4" s="153" t="s">
+      <c r="M4" s="141" t="s">
         <v>25</v>
       </c>
       <c r="N4" s="6" t="s">
         <v>26</v>
       </c>
-      <c r="O4" s="153" t="s">
+      <c r="O4" s="141" t="s">
         <v>27</v>
       </c>
       <c r="P4" s="31" t="s">
         <v>28</v>
       </c>
-      <c r="Q4" s="156" t="s">
+      <c r="Q4" s="144" t="s">
         <v>29</v>
       </c>
-      <c r="R4" s="144" t="s">
+      <c r="R4" s="132" t="s">
         <v>30</v>
       </c>
     </row>
-    <row r="5" spans="1:18" s="2" customFormat="1" ht="15" thickBot="1" x14ac:dyDescent="0.45">
-      <c r="D5" s="138">
+    <row r="5" spans="1:18" s="2" customFormat="1" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="D5" s="126">
         <v>44613</v>
       </c>
-      <c r="E5" s="148">
+      <c r="E5" s="136">
         <f>D5+7</f>
         <v>44620</v>
       </c>
-      <c r="F5" s="151">
+      <c r="F5" s="139">
         <f t="shared" ref="F5:R5" si="0">E5+7</f>
         <v>44627</v>
       </c>
-      <c r="G5" s="151">
+      <c r="G5" s="139">
         <f t="shared" si="0"/>
         <v>44634</v>
       </c>
-      <c r="H5" s="151">
+      <c r="H5" s="139">
         <f t="shared" si="0"/>
         <v>44641</v>
       </c>
-      <c r="I5" s="139">
+      <c r="I5" s="127">
         <f t="shared" si="0"/>
         <v>44648</v>
       </c>
-      <c r="J5" s="140">
+      <c r="J5" s="128">
         <f t="shared" si="0"/>
         <v>44655</v>
       </c>
-      <c r="K5" s="154">
+      <c r="K5" s="142">
         <f t="shared" si="0"/>
         <v>44662</v>
       </c>
-      <c r="L5" s="141">
+      <c r="L5" s="129">
         <f t="shared" si="0"/>
         <v>44669</v>
       </c>
-      <c r="M5" s="154">
+      <c r="M5" s="142">
         <f t="shared" si="0"/>
         <v>44676</v>
       </c>
-      <c r="N5" s="141">
+      <c r="N5" s="129">
         <f t="shared" si="0"/>
         <v>44683</v>
       </c>
-      <c r="O5" s="154">
+      <c r="O5" s="142">
         <f t="shared" si="0"/>
         <v>44690</v>
       </c>
-      <c r="P5" s="142">
+      <c r="P5" s="130">
         <f t="shared" si="0"/>
         <v>44697</v>
       </c>
-      <c r="Q5" s="157">
+      <c r="Q5" s="145">
         <f t="shared" si="0"/>
         <v>44704</v>
       </c>
-      <c r="R5" s="145">
+      <c r="R5" s="133">
         <f t="shared" si="0"/>
         <v>44711</v>
       </c>
     </row>
-    <row r="6" spans="1:18" ht="15" thickBot="1" x14ac:dyDescent="0.45">
+    <row r="6" spans="1:18" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="B6" s="33"/>
       <c r="C6" s="33"/>
-      <c r="D6" s="159"/>
+      <c r="D6" s="147"/>
       <c r="E6" s="26" t="s">
         <v>32</v>
       </c>
@@ -1662,7 +1801,7 @@
         <v>34</v>
       </c>
       <c r="J6" s="7"/>
-      <c r="K6" s="160"/>
+      <c r="K6" s="148"/>
       <c r="L6" s="8" t="s">
         <v>35</v>
       </c>
@@ -1677,456 +1816,456 @@
         <v>37</v>
       </c>
     </row>
-    <row r="7" spans="1:18" ht="15" thickBot="1" x14ac:dyDescent="0.45">
-      <c r="B7" s="110">
+    <row r="7" spans="1:18" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="B7" s="104">
         <v>1</v>
       </c>
-      <c r="C7" s="158" t="s">
+      <c r="C7" s="146" t="s">
         <v>38</v>
       </c>
-      <c r="D7" s="135"/>
-      <c r="E7" s="136"/>
-      <c r="F7" s="136"/>
-      <c r="G7" s="136"/>
-      <c r="H7" s="136"/>
-      <c r="I7" s="136"/>
-      <c r="J7" s="136"/>
-      <c r="K7" s="136"/>
-      <c r="L7" s="136"/>
-      <c r="M7" s="136"/>
-      <c r="N7" s="136"/>
-      <c r="O7" s="136"/>
-      <c r="P7" s="136"/>
-      <c r="Q7" s="136"/>
-      <c r="R7" s="137"/>
-    </row>
-    <row r="8" spans="1:18" x14ac:dyDescent="0.4">
+      <c r="D7" s="153"/>
+      <c r="E7" s="154"/>
+      <c r="F7" s="154"/>
+      <c r="G7" s="154"/>
+      <c r="H7" s="154"/>
+      <c r="I7" s="154"/>
+      <c r="J7" s="154"/>
+      <c r="K7" s="154"/>
+      <c r="L7" s="154"/>
+      <c r="M7" s="154"/>
+      <c r="N7" s="154"/>
+      <c r="O7" s="154"/>
+      <c r="P7" s="154"/>
+      <c r="Q7" s="154"/>
+      <c r="R7" s="155"/>
+    </row>
+    <row r="8" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A8" s="2"/>
-      <c r="B8" s="41">
+      <c r="B8" s="36">
         <v>1.1000000000000001</v>
       </c>
-      <c r="C8" s="42" t="s">
+      <c r="C8" s="37" t="s">
         <v>40</v>
       </c>
-      <c r="D8" s="43"/>
-      <c r="E8" s="44"/>
-      <c r="F8" s="45"/>
-      <c r="G8" s="45"/>
-      <c r="H8" s="45"/>
-      <c r="I8" s="46"/>
-      <c r="J8" s="47"/>
-      <c r="K8" s="160"/>
-      <c r="L8" s="48"/>
-      <c r="M8" s="48"/>
-      <c r="N8" s="48"/>
-      <c r="O8" s="48"/>
-      <c r="P8" s="49"/>
-      <c r="Q8" s="50"/>
-      <c r="R8" s="49"/>
-    </row>
-    <row r="9" spans="1:18" x14ac:dyDescent="0.4">
+      <c r="D8" s="38"/>
+      <c r="E8" s="39"/>
+      <c r="F8" s="40"/>
+      <c r="G8" s="40"/>
+      <c r="H8" s="40"/>
+      <c r="I8" s="41"/>
+      <c r="J8" s="42"/>
+      <c r="K8" s="148"/>
+      <c r="L8" s="43"/>
+      <c r="M8" s="43"/>
+      <c r="N8" s="43"/>
+      <c r="O8" s="43"/>
+      <c r="P8" s="44"/>
+      <c r="Q8" s="45"/>
+      <c r="R8" s="44"/>
+    </row>
+    <row r="9" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A9" s="2"/>
-      <c r="B9" s="51">
+      <c r="B9" s="46">
         <v>1.2</v>
       </c>
-      <c r="C9" s="52" t="s">
+      <c r="C9" s="166" t="s">
+        <v>79</v>
+      </c>
+      <c r="D9" s="47"/>
+      <c r="E9" s="48"/>
+      <c r="F9" s="49"/>
+      <c r="G9" s="49"/>
+      <c r="H9" s="49"/>
+      <c r="I9" s="50"/>
+      <c r="J9" s="48"/>
+      <c r="K9" s="149"/>
+      <c r="L9" s="49"/>
+      <c r="M9" s="49"/>
+      <c r="N9" s="49"/>
+      <c r="O9" s="49"/>
+      <c r="P9" s="50"/>
+      <c r="Q9" s="51"/>
+      <c r="R9" s="52"/>
+    </row>
+    <row r="10" spans="1:18" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A10" s="2"/>
+      <c r="B10" s="53">
+        <v>1.3</v>
+      </c>
+      <c r="C10" s="94" t="s">
         <v>41</v>
       </c>
-      <c r="D9" s="53"/>
-      <c r="E9" s="54"/>
-      <c r="F9" s="55"/>
-      <c r="G9" s="55"/>
-      <c r="H9" s="55"/>
-      <c r="I9" s="56"/>
-      <c r="J9" s="54"/>
-      <c r="K9" s="161"/>
-      <c r="L9" s="55"/>
-      <c r="M9" s="55"/>
-      <c r="N9" s="55"/>
-      <c r="O9" s="55"/>
-      <c r="P9" s="56"/>
-      <c r="Q9" s="57"/>
-      <c r="R9" s="58"/>
-    </row>
-    <row r="10" spans="1:18" ht="15" thickBot="1" x14ac:dyDescent="0.45">
-      <c r="A10" s="2"/>
-      <c r="B10" s="59">
-        <v>1.3</v>
-      </c>
-      <c r="C10" s="100" t="s">
+      <c r="D10" s="95"/>
+      <c r="E10" s="96"/>
+      <c r="F10" s="97"/>
+      <c r="G10" s="97"/>
+      <c r="H10" s="97"/>
+      <c r="I10" s="99"/>
+      <c r="J10" s="100"/>
+      <c r="K10" s="150"/>
+      <c r="L10" s="98"/>
+      <c r="M10" s="101"/>
+      <c r="N10" s="101"/>
+      <c r="O10" s="101"/>
+      <c r="P10" s="102"/>
+      <c r="Q10" s="103"/>
+      <c r="R10" s="102"/>
+    </row>
+    <row r="11" spans="1:18" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="B11" s="104">
+        <v>2</v>
+      </c>
+      <c r="C11" s="105" t="s">
         <v>42</v>
       </c>
-      <c r="D10" s="101"/>
-      <c r="E10" s="102"/>
-      <c r="F10" s="103"/>
-      <c r="G10" s="104"/>
-      <c r="H10" s="104"/>
-      <c r="I10" s="105"/>
-      <c r="J10" s="106"/>
-      <c r="K10" s="162"/>
-      <c r="L10" s="104"/>
-      <c r="M10" s="107"/>
-      <c r="N10" s="107"/>
-      <c r="O10" s="107"/>
-      <c r="P10" s="108"/>
-      <c r="Q10" s="109"/>
-      <c r="R10" s="108"/>
-    </row>
-    <row r="11" spans="1:18" ht="15" thickBot="1" x14ac:dyDescent="0.45">
-      <c r="B11" s="110">
-        <v>2</v>
-      </c>
-      <c r="C11" s="111" t="s">
-        <v>43</v>
-      </c>
-      <c r="D11" s="132"/>
-      <c r="E11" s="133"/>
-      <c r="F11" s="133"/>
-      <c r="G11" s="133"/>
-      <c r="H11" s="133"/>
-      <c r="I11" s="133"/>
-      <c r="J11" s="133"/>
-      <c r="K11" s="133"/>
-      <c r="L11" s="133"/>
-      <c r="M11" s="133"/>
-      <c r="N11" s="133"/>
-      <c r="O11" s="133"/>
-      <c r="P11" s="133"/>
-      <c r="Q11" s="133"/>
-      <c r="R11" s="134"/>
-    </row>
-    <row r="12" spans="1:18" x14ac:dyDescent="0.4">
+      <c r="D11" s="156"/>
+      <c r="E11" s="157"/>
+      <c r="F11" s="157"/>
+      <c r="G11" s="157"/>
+      <c r="H11" s="157"/>
+      <c r="I11" s="157"/>
+      <c r="J11" s="157"/>
+      <c r="K11" s="157"/>
+      <c r="L11" s="157"/>
+      <c r="M11" s="157"/>
+      <c r="N11" s="157"/>
+      <c r="O11" s="157"/>
+      <c r="P11" s="157"/>
+      <c r="Q11" s="157"/>
+      <c r="R11" s="158"/>
+    </row>
+    <row r="12" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A12" s="2"/>
-      <c r="B12" s="41">
+      <c r="B12" s="36">
         <v>2.1</v>
       </c>
-      <c r="C12" s="42" t="s">
+      <c r="C12" s="37" t="s">
+        <v>44</v>
+      </c>
+      <c r="D12" s="106"/>
+      <c r="E12" s="39"/>
+      <c r="F12" s="40"/>
+      <c r="G12" s="40"/>
+      <c r="H12" s="40"/>
+      <c r="I12" s="41"/>
+      <c r="J12" s="39"/>
+      <c r="K12" s="148"/>
+      <c r="L12" s="40"/>
+      <c r="M12" s="40"/>
+      <c r="N12" s="40"/>
+      <c r="O12" s="40"/>
+      <c r="P12" s="41"/>
+      <c r="Q12" s="45"/>
+      <c r="R12" s="44"/>
+    </row>
+    <row r="13" spans="1:18" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A13" s="2"/>
+      <c r="B13" s="68">
+        <v>2.2000000000000002</v>
+      </c>
+      <c r="C13" s="57" t="s">
         <v>45</v>
       </c>
-      <c r="D12" s="112"/>
-      <c r="E12" s="44"/>
-      <c r="F12" s="45"/>
-      <c r="G12" s="45"/>
-      <c r="H12" s="45"/>
-      <c r="I12" s="46"/>
-      <c r="J12" s="44"/>
-      <c r="K12" s="160"/>
-      <c r="L12" s="45"/>
-      <c r="M12" s="45"/>
-      <c r="N12" s="45"/>
-      <c r="O12" s="45"/>
-      <c r="P12" s="46"/>
-      <c r="Q12" s="50"/>
-      <c r="R12" s="49"/>
-    </row>
-    <row r="13" spans="1:18" ht="15" thickBot="1" x14ac:dyDescent="0.45">
-      <c r="A13" s="2"/>
-      <c r="B13" s="74">
-        <v>2.2000000000000002</v>
-      </c>
-      <c r="C13" s="63" t="s">
+      <c r="D13" s="58"/>
+      <c r="E13" s="63"/>
+      <c r="F13" s="61"/>
+      <c r="G13" s="61"/>
+      <c r="H13" s="61"/>
+      <c r="I13" s="62"/>
+      <c r="J13" s="63"/>
+      <c r="K13" s="151"/>
+      <c r="L13" s="60"/>
+      <c r="M13" s="60"/>
+      <c r="N13" s="60"/>
+      <c r="O13" s="60"/>
+      <c r="P13" s="69"/>
+      <c r="Q13" s="70"/>
+      <c r="R13" s="65"/>
+    </row>
+    <row r="14" spans="1:18" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="B14" s="104">
+        <v>3</v>
+      </c>
+      <c r="C14" s="105" t="s">
         <v>46</v>
       </c>
-      <c r="D13" s="64"/>
-      <c r="E13" s="69"/>
-      <c r="F13" s="67"/>
-      <c r="G13" s="67"/>
-      <c r="H13" s="67"/>
-      <c r="I13" s="68"/>
-      <c r="J13" s="69"/>
-      <c r="K13" s="163"/>
-      <c r="L13" s="66"/>
-      <c r="M13" s="66"/>
-      <c r="N13" s="66"/>
-      <c r="O13" s="66"/>
-      <c r="P13" s="75"/>
-      <c r="Q13" s="76"/>
-      <c r="R13" s="71"/>
-    </row>
-    <row r="14" spans="1:18" ht="15" thickBot="1" x14ac:dyDescent="0.45">
-      <c r="B14" s="110">
-        <v>3</v>
-      </c>
-      <c r="C14" s="111" t="s">
-        <v>47</v>
-      </c>
-      <c r="D14" s="132"/>
-      <c r="E14" s="133"/>
-      <c r="F14" s="133"/>
-      <c r="G14" s="133"/>
-      <c r="H14" s="133"/>
-      <c r="I14" s="133"/>
-      <c r="J14" s="133"/>
-      <c r="K14" s="133"/>
-      <c r="L14" s="133"/>
-      <c r="M14" s="133"/>
-      <c r="N14" s="133"/>
-      <c r="O14" s="133"/>
-      <c r="P14" s="133"/>
-      <c r="Q14" s="133"/>
-      <c r="R14" s="134"/>
-    </row>
-    <row r="15" spans="1:18" x14ac:dyDescent="0.4">
+      <c r="D14" s="156"/>
+      <c r="E14" s="157"/>
+      <c r="F14" s="157"/>
+      <c r="G14" s="157"/>
+      <c r="H14" s="157"/>
+      <c r="I14" s="157"/>
+      <c r="J14" s="157"/>
+      <c r="K14" s="157"/>
+      <c r="L14" s="157"/>
+      <c r="M14" s="157"/>
+      <c r="N14" s="157"/>
+      <c r="O14" s="157"/>
+      <c r="P14" s="157"/>
+      <c r="Q14" s="157"/>
+      <c r="R14" s="158"/>
+    </row>
+    <row r="15" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A15" s="2"/>
-      <c r="B15" s="41">
+      <c r="B15" s="36">
         <v>3.1</v>
       </c>
-      <c r="C15" s="42" t="s">
+      <c r="C15" s="37" t="s">
+        <v>48</v>
+      </c>
+      <c r="D15" s="66"/>
+      <c r="E15" s="39"/>
+      <c r="F15" s="40"/>
+      <c r="G15" s="40"/>
+      <c r="H15" s="40"/>
+      <c r="I15" s="41"/>
+      <c r="J15" s="39"/>
+      <c r="K15" s="148"/>
+      <c r="L15" s="107"/>
+      <c r="M15" s="107"/>
+      <c r="N15" s="107"/>
+      <c r="O15" s="107"/>
+      <c r="P15" s="108"/>
+      <c r="Q15" s="109"/>
+      <c r="R15" s="44"/>
+    </row>
+    <row r="16" spans="1:18" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A16" s="2"/>
+      <c r="B16" s="68">
+        <v>3.2</v>
+      </c>
+      <c r="C16" s="167" t="s">
+        <v>74</v>
+      </c>
+      <c r="D16" s="110"/>
+      <c r="E16" s="63"/>
+      <c r="F16" s="60"/>
+      <c r="G16" s="60"/>
+      <c r="H16" s="60"/>
+      <c r="I16" s="69"/>
+      <c r="J16" s="59"/>
+      <c r="K16" s="151"/>
+      <c r="L16" s="60"/>
+      <c r="M16" s="60"/>
+      <c r="N16" s="60"/>
+      <c r="O16" s="60"/>
+      <c r="P16" s="69"/>
+      <c r="Q16" s="70"/>
+      <c r="R16" s="65"/>
+    </row>
+    <row r="17" spans="1:28" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="B17" s="104">
+        <v>4</v>
+      </c>
+      <c r="C17" s="105" t="s">
         <v>49</v>
       </c>
-      <c r="D15" s="72"/>
-      <c r="E15" s="44"/>
-      <c r="F15" s="45"/>
-      <c r="G15" s="45"/>
-      <c r="H15" s="45"/>
-      <c r="I15" s="46"/>
-      <c r="J15" s="44"/>
-      <c r="K15" s="160"/>
-      <c r="L15" s="113"/>
-      <c r="M15" s="113"/>
-      <c r="N15" s="113"/>
-      <c r="O15" s="113"/>
-      <c r="P15" s="114"/>
-      <c r="Q15" s="115"/>
-      <c r="R15" s="49"/>
-    </row>
-    <row r="16" spans="1:18" ht="15" thickBot="1" x14ac:dyDescent="0.45">
-      <c r="A16" s="2"/>
-      <c r="B16" s="74">
-        <v>3.2</v>
-      </c>
-      <c r="C16" s="63" t="s">
-        <v>50</v>
-      </c>
-      <c r="D16" s="116"/>
-      <c r="E16" s="69"/>
-      <c r="F16" s="66"/>
-      <c r="G16" s="66"/>
-      <c r="H16" s="66"/>
-      <c r="I16" s="75"/>
-      <c r="J16" s="65"/>
-      <c r="K16" s="163"/>
-      <c r="L16" s="66"/>
-      <c r="M16" s="66"/>
-      <c r="N16" s="66"/>
-      <c r="O16" s="66"/>
-      <c r="P16" s="75"/>
-      <c r="Q16" s="76"/>
-      <c r="R16" s="71"/>
-    </row>
-    <row r="17" spans="1:28" ht="15" thickBot="1" x14ac:dyDescent="0.45">
-      <c r="B17" s="110">
-        <v>4</v>
-      </c>
-      <c r="C17" s="111" t="s">
-        <v>51</v>
-      </c>
-      <c r="D17" s="132"/>
-      <c r="E17" s="133"/>
-      <c r="F17" s="133"/>
-      <c r="G17" s="133"/>
-      <c r="H17" s="133"/>
-      <c r="I17" s="133"/>
-      <c r="J17" s="133"/>
-      <c r="K17" s="133"/>
-      <c r="L17" s="133"/>
-      <c r="M17" s="133"/>
-      <c r="N17" s="133"/>
-      <c r="O17" s="133"/>
-      <c r="P17" s="133"/>
-      <c r="Q17" s="133"/>
-      <c r="R17" s="134"/>
-    </row>
-    <row r="18" spans="1:28" x14ac:dyDescent="0.4">
+      <c r="D17" s="156"/>
+      <c r="E17" s="157"/>
+      <c r="F17" s="157"/>
+      <c r="G17" s="157"/>
+      <c r="H17" s="157"/>
+      <c r="I17" s="157"/>
+      <c r="J17" s="157"/>
+      <c r="K17" s="157"/>
+      <c r="L17" s="157"/>
+      <c r="M17" s="157"/>
+      <c r="N17" s="157"/>
+      <c r="O17" s="157"/>
+      <c r="P17" s="157"/>
+      <c r="Q17" s="157"/>
+      <c r="R17" s="158"/>
+    </row>
+    <row r="18" spans="1:28" x14ac:dyDescent="0.25">
       <c r="A18" s="2"/>
-      <c r="B18" s="41">
+      <c r="B18" s="36">
         <v>4.0999999999999996</v>
       </c>
-      <c r="C18" s="42" t="s">
-        <v>53</v>
-      </c>
-      <c r="D18" s="72"/>
-      <c r="E18" s="47"/>
-      <c r="F18" s="45"/>
-      <c r="G18" s="45"/>
-      <c r="H18" s="45"/>
-      <c r="I18" s="46"/>
-      <c r="J18" s="44"/>
-      <c r="K18" s="160"/>
-      <c r="L18" s="113"/>
-      <c r="M18" s="113"/>
-      <c r="N18" s="113"/>
-      <c r="O18" s="113"/>
-      <c r="P18" s="114"/>
-      <c r="Q18" s="115"/>
-      <c r="R18" s="49"/>
-    </row>
-    <row r="19" spans="1:28" x14ac:dyDescent="0.4">
+      <c r="C18" s="168" t="s">
+        <v>80</v>
+      </c>
+      <c r="D18" s="66"/>
+      <c r="E18" s="42"/>
+      <c r="F18" s="40"/>
+      <c r="G18" s="40"/>
+      <c r="H18" s="40"/>
+      <c r="I18" s="41"/>
+      <c r="J18" s="39"/>
+      <c r="K18" s="148"/>
+      <c r="L18" s="107"/>
+      <c r="M18" s="107"/>
+      <c r="N18" s="107"/>
+      <c r="O18" s="107"/>
+      <c r="P18" s="108"/>
+      <c r="Q18" s="109"/>
+      <c r="R18" s="44"/>
+    </row>
+    <row r="19" spans="1:28" x14ac:dyDescent="0.25">
       <c r="A19" s="2"/>
-      <c r="B19" s="51">
+      <c r="B19" s="46">
         <v>4.2</v>
       </c>
-      <c r="C19" s="52" t="s">
-        <v>55</v>
-      </c>
-      <c r="D19" s="77"/>
-      <c r="E19" s="61"/>
-      <c r="F19" s="78"/>
-      <c r="G19" s="78"/>
-      <c r="H19" s="55"/>
-      <c r="I19" s="56"/>
-      <c r="J19" s="54"/>
-      <c r="K19" s="161"/>
-      <c r="L19" s="78"/>
-      <c r="M19" s="78"/>
-      <c r="N19" s="78"/>
-      <c r="O19" s="78"/>
-      <c r="P19" s="79"/>
-      <c r="Q19" s="80"/>
-      <c r="R19" s="58"/>
-    </row>
-    <row r="20" spans="1:28" x14ac:dyDescent="0.4">
+      <c r="C19" s="166" t="s">
+        <v>81</v>
+      </c>
+      <c r="D19" s="71"/>
+      <c r="E19" s="55"/>
+      <c r="F19" s="72"/>
+      <c r="G19" s="72"/>
+      <c r="H19" s="49"/>
+      <c r="I19" s="50"/>
+      <c r="J19" s="48"/>
+      <c r="K19" s="149"/>
+      <c r="L19" s="72"/>
+      <c r="M19" s="72"/>
+      <c r="N19" s="72"/>
+      <c r="O19" s="72"/>
+      <c r="P19" s="73"/>
+      <c r="Q19" s="74"/>
+      <c r="R19" s="52"/>
+    </row>
+    <row r="20" spans="1:28" x14ac:dyDescent="0.25">
       <c r="A20" s="2"/>
-      <c r="B20" s="51">
+      <c r="B20" s="46">
         <v>4.3</v>
       </c>
-      <c r="C20" s="52" t="s">
+      <c r="C20" s="166" t="s">
+        <v>82</v>
+      </c>
+      <c r="D20" s="71"/>
+      <c r="E20" s="55"/>
+      <c r="F20" s="49"/>
+      <c r="G20" s="49"/>
+      <c r="H20" s="49"/>
+      <c r="I20" s="73"/>
+      <c r="J20" s="55"/>
+      <c r="K20" s="149"/>
+      <c r="L20" s="72"/>
+      <c r="M20" s="72"/>
+      <c r="N20" s="72"/>
+      <c r="O20" s="72"/>
+      <c r="P20" s="73"/>
+      <c r="Q20" s="74"/>
+      <c r="R20" s="52"/>
+    </row>
+    <row r="21" spans="1:28" x14ac:dyDescent="0.25">
+      <c r="A21" s="2"/>
+      <c r="B21" s="46">
+        <v>4.4000000000000004</v>
+      </c>
+      <c r="C21" s="166" t="s">
+        <v>83</v>
+      </c>
+      <c r="D21" s="71"/>
+      <c r="E21" s="55"/>
+      <c r="F21" s="72"/>
+      <c r="G21" s="72"/>
+      <c r="H21" s="49"/>
+      <c r="I21" s="50"/>
+      <c r="J21" s="48"/>
+      <c r="K21" s="149"/>
+      <c r="L21" s="49"/>
+      <c r="M21" s="49"/>
+      <c r="N21" s="49"/>
+      <c r="O21" s="49"/>
+      <c r="P21" s="50"/>
+      <c r="Q21" s="74"/>
+      <c r="R21" s="52"/>
+    </row>
+    <row r="22" spans="1:28" x14ac:dyDescent="0.25">
+      <c r="A22" s="2"/>
+      <c r="B22" s="46">
+        <v>4.5</v>
+      </c>
+      <c r="C22" s="166" t="s">
+        <v>75</v>
+      </c>
+      <c r="D22" s="71"/>
+      <c r="E22" s="55"/>
+      <c r="F22" s="49"/>
+      <c r="G22" s="49"/>
+      <c r="H22" s="49"/>
+      <c r="I22" s="73"/>
+      <c r="J22" s="55"/>
+      <c r="K22" s="149"/>
+      <c r="L22" s="72"/>
+      <c r="M22" s="72"/>
+      <c r="N22" s="72"/>
+      <c r="O22" s="72"/>
+      <c r="P22" s="73"/>
+      <c r="Q22" s="74"/>
+      <c r="R22" s="52"/>
+    </row>
+    <row r="23" spans="1:28" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A23" s="2"/>
+      <c r="B23" s="68">
+        <v>4.5999999999999996</v>
+      </c>
+      <c r="C23" s="167" t="s">
+        <v>76</v>
+      </c>
+      <c r="D23" s="110"/>
+      <c r="E23" s="63"/>
+      <c r="F23" s="61"/>
+      <c r="G23" s="60"/>
+      <c r="H23" s="60"/>
+      <c r="I23" s="69"/>
+      <c r="J23" s="59"/>
+      <c r="K23" s="151"/>
+      <c r="L23" s="60"/>
+      <c r="M23" s="60"/>
+      <c r="N23" s="60"/>
+      <c r="O23" s="60"/>
+      <c r="P23" s="69"/>
+      <c r="Q23" s="70"/>
+      <c r="R23" s="65"/>
+    </row>
+    <row r="24" spans="1:28" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="B24" s="104">
+        <v>5</v>
+      </c>
+      <c r="C24" s="105" t="s">
         <v>57</v>
       </c>
-      <c r="D20" s="77"/>
-      <c r="E20" s="61"/>
-      <c r="F20" s="55"/>
-      <c r="G20" s="55"/>
-      <c r="H20" s="55"/>
-      <c r="I20" s="79"/>
-      <c r="J20" s="61"/>
-      <c r="K20" s="161"/>
-      <c r="L20" s="78"/>
-      <c r="M20" s="78"/>
-      <c r="N20" s="78"/>
-      <c r="O20" s="78"/>
-      <c r="P20" s="79"/>
-      <c r="Q20" s="80"/>
-      <c r="R20" s="58"/>
-    </row>
-    <row r="21" spans="1:28" x14ac:dyDescent="0.4">
-      <c r="A21" s="2"/>
-      <c r="B21" s="51">
-        <v>4.4000000000000004</v>
-      </c>
-      <c r="C21" s="52" t="s">
-        <v>59</v>
-      </c>
-      <c r="D21" s="77"/>
-      <c r="E21" s="61"/>
-      <c r="F21" s="78"/>
-      <c r="G21" s="78"/>
-      <c r="H21" s="55"/>
-      <c r="I21" s="56"/>
-      <c r="J21" s="54"/>
-      <c r="K21" s="161"/>
-      <c r="L21" s="55"/>
-      <c r="M21" s="55"/>
-      <c r="N21" s="55"/>
-      <c r="O21" s="55"/>
-      <c r="P21" s="56"/>
-      <c r="Q21" s="80"/>
-      <c r="R21" s="58"/>
-    </row>
-    <row r="22" spans="1:28" x14ac:dyDescent="0.4">
-      <c r="A22" s="2"/>
-      <c r="B22" s="51">
-        <v>4.5</v>
-      </c>
-      <c r="C22" s="52" t="s">
-        <v>61</v>
-      </c>
-      <c r="D22" s="77"/>
-      <c r="E22" s="61"/>
-      <c r="F22" s="55"/>
-      <c r="G22" s="55"/>
-      <c r="H22" s="55"/>
-      <c r="I22" s="79"/>
-      <c r="J22" s="61"/>
-      <c r="K22" s="161"/>
-      <c r="L22" s="78"/>
-      <c r="M22" s="78"/>
-      <c r="N22" s="78"/>
-      <c r="O22" s="78"/>
-      <c r="P22" s="79"/>
-      <c r="Q22" s="80"/>
-      <c r="R22" s="58"/>
-    </row>
-    <row r="23" spans="1:28" ht="15" thickBot="1" x14ac:dyDescent="0.45">
-      <c r="A23" s="2"/>
-      <c r="B23" s="74">
-        <v>4.5999999999999996</v>
-      </c>
-      <c r="C23" s="63" t="s">
-        <v>63</v>
-      </c>
-      <c r="D23" s="116"/>
-      <c r="E23" s="69"/>
-      <c r="F23" s="67"/>
-      <c r="G23" s="66"/>
-      <c r="H23" s="66"/>
-      <c r="I23" s="75"/>
-      <c r="J23" s="65"/>
-      <c r="K23" s="163"/>
-      <c r="L23" s="66"/>
-      <c r="M23" s="66"/>
-      <c r="N23" s="66"/>
-      <c r="O23" s="66"/>
-      <c r="P23" s="75"/>
-      <c r="Q23" s="76"/>
-      <c r="R23" s="71"/>
-    </row>
-    <row r="24" spans="1:28" ht="15" thickBot="1" x14ac:dyDescent="0.45">
-      <c r="B24" s="110">
-        <v>5</v>
-      </c>
-      <c r="C24" s="111" t="s">
-        <v>65</v>
-      </c>
-      <c r="D24" s="132"/>
-      <c r="E24" s="133"/>
-      <c r="F24" s="133"/>
-      <c r="G24" s="133"/>
-      <c r="H24" s="133"/>
-      <c r="I24" s="133"/>
-      <c r="J24" s="133"/>
-      <c r="K24" s="133"/>
-      <c r="L24" s="133"/>
-      <c r="M24" s="133"/>
-      <c r="N24" s="133"/>
-      <c r="O24" s="133"/>
-      <c r="P24" s="133"/>
-      <c r="Q24" s="133"/>
-      <c r="R24" s="134"/>
-    </row>
-    <row r="25" spans="1:28" x14ac:dyDescent="0.4">
+      <c r="D24" s="156"/>
+      <c r="E24" s="157"/>
+      <c r="F24" s="157"/>
+      <c r="G24" s="157"/>
+      <c r="H24" s="157"/>
+      <c r="I24" s="157"/>
+      <c r="J24" s="157"/>
+      <c r="K24" s="157"/>
+      <c r="L24" s="157"/>
+      <c r="M24" s="157"/>
+      <c r="N24" s="157"/>
+      <c r="O24" s="157"/>
+      <c r="P24" s="157"/>
+      <c r="Q24" s="157"/>
+      <c r="R24" s="158"/>
+    </row>
+    <row r="25" spans="1:28" x14ac:dyDescent="0.25">
       <c r="A25" s="2"/>
-      <c r="B25" s="41">
+      <c r="B25" s="36">
         <v>5.0999999999999996</v>
       </c>
-      <c r="C25" s="42" t="s">
-        <v>66</v>
-      </c>
-      <c r="D25" s="72"/>
-      <c r="E25" s="117"/>
-      <c r="F25" s="45"/>
-      <c r="G25" s="45"/>
-      <c r="H25" s="45"/>
-      <c r="I25" s="46"/>
-      <c r="J25" s="44"/>
-      <c r="K25" s="160"/>
-      <c r="L25" s="113"/>
-      <c r="M25" s="113"/>
-      <c r="N25" s="113"/>
-      <c r="O25" s="113"/>
-      <c r="P25" s="46"/>
-      <c r="Q25" s="118"/>
-      <c r="R25" s="114"/>
+      <c r="C25" s="168" t="s">
+        <v>84</v>
+      </c>
+      <c r="D25" s="66"/>
+      <c r="E25" s="111"/>
+      <c r="F25" s="40"/>
+      <c r="G25" s="40"/>
+      <c r="H25" s="40"/>
+      <c r="I25" s="41"/>
+      <c r="J25" s="39"/>
+      <c r="K25" s="148"/>
+      <c r="L25" s="107"/>
+      <c r="M25" s="107"/>
+      <c r="N25" s="107"/>
+      <c r="O25" s="107"/>
+      <c r="P25" s="41"/>
+      <c r="Q25" s="112"/>
+      <c r="R25" s="108"/>
       <c r="S25" s="4"/>
       <c r="T25" s="4"/>
       <c r="U25" s="4"/>
@@ -2138,29 +2277,29 @@
       <c r="AA25" s="4"/>
       <c r="AB25" s="4"/>
     </row>
-    <row r="26" spans="1:28" x14ac:dyDescent="0.4">
+    <row r="26" spans="1:28" x14ac:dyDescent="0.25">
       <c r="A26" s="2"/>
-      <c r="B26" s="51">
+      <c r="B26" s="46">
         <v>5.2</v>
       </c>
-      <c r="C26" s="52" t="s">
-        <v>67</v>
-      </c>
-      <c r="D26" s="77"/>
-      <c r="E26" s="82"/>
-      <c r="F26" s="62"/>
-      <c r="G26" s="78"/>
-      <c r="H26" s="55"/>
-      <c r="I26" s="56"/>
-      <c r="J26" s="54"/>
-      <c r="K26" s="161"/>
-      <c r="L26" s="78"/>
-      <c r="M26" s="78"/>
-      <c r="N26" s="78"/>
-      <c r="O26" s="78"/>
-      <c r="P26" s="56"/>
-      <c r="Q26" s="57"/>
-      <c r="R26" s="79"/>
+      <c r="C26" s="166" t="s">
+        <v>85</v>
+      </c>
+      <c r="D26" s="71"/>
+      <c r="E26" s="76"/>
+      <c r="F26" s="56"/>
+      <c r="G26" s="72"/>
+      <c r="H26" s="49"/>
+      <c r="I26" s="50"/>
+      <c r="J26" s="48"/>
+      <c r="K26" s="149"/>
+      <c r="L26" s="72"/>
+      <c r="M26" s="72"/>
+      <c r="N26" s="72"/>
+      <c r="O26" s="72"/>
+      <c r="P26" s="50"/>
+      <c r="Q26" s="51"/>
+      <c r="R26" s="73"/>
       <c r="S26" s="4"/>
       <c r="T26" s="4"/>
       <c r="U26" s="4"/>
@@ -2172,29 +2311,29 @@
       <c r="AA26" s="4"/>
       <c r="AB26" s="4"/>
     </row>
-    <row r="27" spans="1:28" x14ac:dyDescent="0.4">
+    <row r="27" spans="1:28" x14ac:dyDescent="0.25">
       <c r="A27" s="2"/>
-      <c r="B27" s="51">
+      <c r="B27" s="46">
         <v>5.3</v>
       </c>
-      <c r="C27" s="52" t="s">
-        <v>68</v>
-      </c>
-      <c r="D27" s="77"/>
-      <c r="E27" s="82"/>
-      <c r="F27" s="55"/>
-      <c r="G27" s="55"/>
-      <c r="H27" s="55"/>
-      <c r="I27" s="79"/>
-      <c r="J27" s="61"/>
-      <c r="K27" s="161"/>
-      <c r="L27" s="78"/>
-      <c r="M27" s="78"/>
-      <c r="N27" s="78"/>
-      <c r="O27" s="78"/>
-      <c r="P27" s="56"/>
-      <c r="Q27" s="57"/>
-      <c r="R27" s="79"/>
+      <c r="C27" s="166" t="s">
+        <v>86</v>
+      </c>
+      <c r="D27" s="71"/>
+      <c r="E27" s="76"/>
+      <c r="F27" s="49"/>
+      <c r="G27" s="49"/>
+      <c r="H27" s="49"/>
+      <c r="I27" s="73"/>
+      <c r="J27" s="55"/>
+      <c r="K27" s="149"/>
+      <c r="L27" s="72"/>
+      <c r="M27" s="72"/>
+      <c r="N27" s="72"/>
+      <c r="O27" s="72"/>
+      <c r="P27" s="50"/>
+      <c r="Q27" s="51"/>
+      <c r="R27" s="73"/>
       <c r="S27" s="4"/>
       <c r="T27" s="4"/>
       <c r="U27" s="4"/>
@@ -2206,29 +2345,29 @@
       <c r="AA27" s="4"/>
       <c r="AB27" s="4"/>
     </row>
-    <row r="28" spans="1:28" x14ac:dyDescent="0.4">
+    <row r="28" spans="1:28" x14ac:dyDescent="0.25">
       <c r="A28" s="2"/>
-      <c r="B28" s="51">
+      <c r="B28" s="46">
         <v>5.4</v>
       </c>
-      <c r="C28" s="52" t="s">
-        <v>69</v>
-      </c>
-      <c r="D28" s="77"/>
-      <c r="E28" s="82"/>
-      <c r="F28" s="62"/>
-      <c r="G28" s="78"/>
-      <c r="H28" s="55"/>
-      <c r="I28" s="56"/>
-      <c r="J28" s="54"/>
-      <c r="K28" s="161"/>
-      <c r="L28" s="55"/>
-      <c r="M28" s="55"/>
-      <c r="N28" s="55"/>
-      <c r="O28" s="55"/>
-      <c r="P28" s="56"/>
-      <c r="Q28" s="57"/>
-      <c r="R28" s="79"/>
+      <c r="C28" s="166" t="s">
+        <v>87</v>
+      </c>
+      <c r="D28" s="71"/>
+      <c r="E28" s="76"/>
+      <c r="F28" s="56"/>
+      <c r="G28" s="72"/>
+      <c r="H28" s="49"/>
+      <c r="I28" s="50"/>
+      <c r="J28" s="48"/>
+      <c r="K28" s="149"/>
+      <c r="L28" s="49"/>
+      <c r="M28" s="49"/>
+      <c r="N28" s="49"/>
+      <c r="O28" s="49"/>
+      <c r="P28" s="50"/>
+      <c r="Q28" s="51"/>
+      <c r="R28" s="73"/>
       <c r="S28" s="4"/>
       <c r="T28" s="4"/>
       <c r="U28" s="4"/>
@@ -2240,29 +2379,29 @@
       <c r="AA28" s="4"/>
       <c r="AB28" s="4"/>
     </row>
-    <row r="29" spans="1:28" x14ac:dyDescent="0.4">
+    <row r="29" spans="1:28" x14ac:dyDescent="0.25">
       <c r="A29" s="2"/>
-      <c r="B29" s="51">
+      <c r="B29" s="46">
         <v>5.5</v>
       </c>
-      <c r="C29" s="52" t="s">
-        <v>70</v>
-      </c>
-      <c r="D29" s="77"/>
-      <c r="E29" s="82"/>
-      <c r="F29" s="55"/>
-      <c r="G29" s="55"/>
-      <c r="H29" s="55"/>
-      <c r="I29" s="79"/>
-      <c r="J29" s="61"/>
-      <c r="K29" s="161"/>
-      <c r="L29" s="78"/>
-      <c r="M29" s="78"/>
-      <c r="N29" s="78"/>
-      <c r="O29" s="78"/>
-      <c r="P29" s="56"/>
-      <c r="Q29" s="57"/>
-      <c r="R29" s="79"/>
+      <c r="C29" s="166" t="s">
+        <v>77</v>
+      </c>
+      <c r="D29" s="71"/>
+      <c r="E29" s="76"/>
+      <c r="F29" s="49"/>
+      <c r="G29" s="49"/>
+      <c r="H29" s="49"/>
+      <c r="I29" s="49"/>
+      <c r="J29" s="55"/>
+      <c r="K29" s="149"/>
+      <c r="L29" s="72"/>
+      <c r="M29" s="72"/>
+      <c r="N29" s="72"/>
+      <c r="O29" s="72"/>
+      <c r="P29" s="50"/>
+      <c r="Q29" s="51"/>
+      <c r="R29" s="73"/>
       <c r="S29" s="4"/>
       <c r="T29" s="4"/>
       <c r="U29" s="4"/>
@@ -2274,29 +2413,29 @@
       <c r="AA29" s="4"/>
       <c r="AB29" s="4"/>
     </row>
-    <row r="30" spans="1:28" x14ac:dyDescent="0.4">
+    <row r="30" spans="1:28" x14ac:dyDescent="0.25">
       <c r="A30" s="2"/>
-      <c r="B30" s="51">
+      <c r="B30" s="46">
         <v>5.6</v>
       </c>
-      <c r="C30" s="52" t="s">
-        <v>71</v>
-      </c>
-      <c r="D30" s="77"/>
-      <c r="E30" s="82"/>
-      <c r="F30" s="62"/>
-      <c r="G30" s="55"/>
-      <c r="H30" s="55"/>
-      <c r="I30" s="56"/>
-      <c r="J30" s="54"/>
-      <c r="K30" s="161"/>
-      <c r="L30" s="55"/>
-      <c r="M30" s="55"/>
-      <c r="N30" s="55"/>
-      <c r="O30" s="55"/>
-      <c r="P30" s="56"/>
-      <c r="Q30" s="57"/>
-      <c r="R30" s="79"/>
+      <c r="C30" s="166" t="s">
+        <v>78</v>
+      </c>
+      <c r="D30" s="71"/>
+      <c r="E30" s="76"/>
+      <c r="F30" s="56"/>
+      <c r="G30" s="49"/>
+      <c r="H30" s="49"/>
+      <c r="I30" s="50"/>
+      <c r="J30" s="48"/>
+      <c r="K30" s="149"/>
+      <c r="L30" s="49"/>
+      <c r="M30" s="49"/>
+      <c r="N30" s="49"/>
+      <c r="O30" s="49"/>
+      <c r="P30" s="50"/>
+      <c r="Q30" s="51"/>
+      <c r="R30" s="73"/>
       <c r="S30" s="4"/>
       <c r="T30" s="4"/>
       <c r="U30" s="4"/>
@@ -2308,29 +2447,29 @@
       <c r="AA30" s="4"/>
       <c r="AB30" s="4"/>
     </row>
-    <row r="31" spans="1:28" ht="15" thickBot="1" x14ac:dyDescent="0.45">
+    <row r="31" spans="1:28" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A31" s="2"/>
-      <c r="B31" s="74">
+      <c r="B31" s="68">
         <v>5.7</v>
       </c>
-      <c r="C31" s="63" t="s">
-        <v>72</v>
-      </c>
-      <c r="D31" s="116"/>
-      <c r="E31" s="119"/>
-      <c r="F31" s="70"/>
-      <c r="G31" s="67"/>
-      <c r="H31" s="67"/>
-      <c r="I31" s="68"/>
-      <c r="J31" s="69"/>
-      <c r="K31" s="163"/>
-      <c r="L31" s="67"/>
-      <c r="M31" s="67"/>
-      <c r="N31" s="67"/>
-      <c r="O31" s="67"/>
-      <c r="P31" s="75"/>
-      <c r="Q31" s="76"/>
-      <c r="R31" s="75"/>
+      <c r="C31" s="57" t="s">
+        <v>58</v>
+      </c>
+      <c r="D31" s="110"/>
+      <c r="E31" s="113"/>
+      <c r="F31" s="64"/>
+      <c r="G31" s="61"/>
+      <c r="H31" s="61"/>
+      <c r="I31" s="62"/>
+      <c r="J31" s="63"/>
+      <c r="K31" s="151"/>
+      <c r="L31" s="61"/>
+      <c r="M31" s="61"/>
+      <c r="N31" s="61"/>
+      <c r="O31" s="61"/>
+      <c r="P31" s="69"/>
+      <c r="Q31" s="70"/>
+      <c r="R31" s="69"/>
       <c r="S31" s="4"/>
       <c r="T31" s="4"/>
       <c r="U31" s="4"/>
@@ -2342,36 +2481,36 @@
       <c r="AA31" s="4"/>
       <c r="AB31" s="4"/>
     </row>
-    <row r="32" spans="1:28" ht="15" thickBot="1" x14ac:dyDescent="0.45">
-      <c r="B32" s="110">
+    <row r="32" spans="1:28" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="B32" s="104">
         <v>6</v>
       </c>
-      <c r="C32" s="111" t="s">
-        <v>73</v>
-      </c>
-      <c r="D32" s="132"/>
-      <c r="E32" s="133"/>
-      <c r="F32" s="133"/>
-      <c r="G32" s="133"/>
-      <c r="H32" s="133"/>
-      <c r="I32" s="133"/>
-      <c r="J32" s="133"/>
-      <c r="K32" s="133"/>
-      <c r="L32" s="133"/>
-      <c r="M32" s="133"/>
-      <c r="N32" s="133"/>
-      <c r="O32" s="133"/>
-      <c r="P32" s="133"/>
-      <c r="Q32" s="133"/>
-      <c r="R32" s="134"/>
-    </row>
-    <row r="33" spans="1:31" ht="15" thickBot="1" x14ac:dyDescent="0.45">
+      <c r="C32" s="105" t="s">
+        <v>59</v>
+      </c>
+      <c r="D32" s="156"/>
+      <c r="E32" s="157"/>
+      <c r="F32" s="157"/>
+      <c r="G32" s="157"/>
+      <c r="H32" s="157"/>
+      <c r="I32" s="157"/>
+      <c r="J32" s="157"/>
+      <c r="K32" s="157"/>
+      <c r="L32" s="157"/>
+      <c r="M32" s="157"/>
+      <c r="N32" s="157"/>
+      <c r="O32" s="157"/>
+      <c r="P32" s="157"/>
+      <c r="Q32" s="157"/>
+      <c r="R32" s="158"/>
+    </row>
+    <row r="33" spans="1:31" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A33" s="2"/>
-      <c r="B33" s="35">
+      <c r="B33" s="34">
         <v>6.1</v>
       </c>
-      <c r="C33" s="34" t="s">
-        <v>74</v>
+      <c r="C33" s="169" t="s">
+        <v>88</v>
       </c>
       <c r="D33" s="22"/>
       <c r="E33" s="16"/>
@@ -2380,7 +2519,7 @@
       <c r="H33" s="12"/>
       <c r="I33" s="17"/>
       <c r="J33" s="11"/>
-      <c r="K33" s="164"/>
+      <c r="K33" s="152"/>
       <c r="L33" s="12"/>
       <c r="M33" s="12"/>
       <c r="N33" s="12"/>
@@ -2402,35 +2541,35 @@
       <c r="AD33" s="4"/>
       <c r="AE33" s="4"/>
     </row>
-    <row r="34" spans="1:31" ht="15" thickBot="1" x14ac:dyDescent="0.45">
-      <c r="B34" s="110">
+    <row r="34" spans="1:31" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="B34" s="104">
         <v>7</v>
       </c>
-      <c r="C34" s="111" t="s">
-        <v>75</v>
-      </c>
-      <c r="D34" s="132"/>
-      <c r="E34" s="133"/>
-      <c r="F34" s="133"/>
-      <c r="G34" s="133"/>
-      <c r="H34" s="133"/>
-      <c r="I34" s="133"/>
-      <c r="J34" s="133"/>
-      <c r="K34" s="133"/>
-      <c r="L34" s="133"/>
-      <c r="M34" s="133"/>
-      <c r="N34" s="133"/>
-      <c r="O34" s="133"/>
-      <c r="P34" s="133"/>
-      <c r="Q34" s="133"/>
-      <c r="R34" s="134"/>
-    </row>
-    <row r="35" spans="1:31" s="4" customFormat="1" ht="15" thickBot="1" x14ac:dyDescent="0.45">
-      <c r="B35" s="36">
+      <c r="C34" s="105" t="s">
+        <v>60</v>
+      </c>
+      <c r="D34" s="156"/>
+      <c r="E34" s="157"/>
+      <c r="F34" s="157"/>
+      <c r="G34" s="157"/>
+      <c r="H34" s="157"/>
+      <c r="I34" s="157"/>
+      <c r="J34" s="157"/>
+      <c r="K34" s="157"/>
+      <c r="L34" s="157"/>
+      <c r="M34" s="157"/>
+      <c r="N34" s="157"/>
+      <c r="O34" s="157"/>
+      <c r="P34" s="157"/>
+      <c r="Q34" s="157"/>
+      <c r="R34" s="158"/>
+    </row>
+    <row r="35" spans="1:31" s="4" customFormat="1" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="B35" s="35">
         <v>7.1</v>
       </c>
-      <c r="C35" s="121" t="s">
-        <v>83</v>
+      <c r="C35" s="115" t="s">
+        <v>68</v>
       </c>
       <c r="D35" s="21"/>
       <c r="E35" s="15"/>
@@ -2439,7 +2578,7 @@
       <c r="H35" s="12"/>
       <c r="I35" s="17"/>
       <c r="J35" s="11"/>
-      <c r="K35" s="164"/>
+      <c r="K35" s="152"/>
       <c r="L35" s="12"/>
       <c r="M35" s="12"/>
       <c r="N35" s="12"/>
@@ -2448,340 +2587,341 @@
       <c r="Q35" s="18"/>
       <c r="R35" s="17"/>
     </row>
-    <row r="36" spans="1:31" ht="15" thickBot="1" x14ac:dyDescent="0.45">
-      <c r="B36" s="110">
+    <row r="36" spans="1:31" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="B36" s="104">
         <v>8</v>
       </c>
-      <c r="C36" s="111" t="s">
-        <v>76</v>
-      </c>
-      <c r="D36" s="132"/>
-      <c r="E36" s="133"/>
-      <c r="F36" s="133"/>
-      <c r="G36" s="133"/>
-      <c r="H36" s="133"/>
-      <c r="I36" s="133"/>
-      <c r="J36" s="133"/>
-      <c r="K36" s="133"/>
-      <c r="L36" s="133"/>
-      <c r="M36" s="133"/>
-      <c r="N36" s="133"/>
-      <c r="O36" s="133"/>
-      <c r="P36" s="133"/>
-      <c r="Q36" s="133"/>
-      <c r="R36" s="134"/>
-    </row>
-    <row r="37" spans="1:31" s="4" customFormat="1" x14ac:dyDescent="0.4">
-      <c r="B37" s="120">
+      <c r="C36" s="105" t="s">
+        <v>61</v>
+      </c>
+      <c r="D36" s="156"/>
+      <c r="E36" s="157"/>
+      <c r="F36" s="157"/>
+      <c r="G36" s="157"/>
+      <c r="H36" s="157"/>
+      <c r="I36" s="157"/>
+      <c r="J36" s="157"/>
+      <c r="K36" s="157"/>
+      <c r="L36" s="157"/>
+      <c r="M36" s="157"/>
+      <c r="N36" s="157"/>
+      <c r="O36" s="157"/>
+      <c r="P36" s="157"/>
+      <c r="Q36" s="157"/>
+      <c r="R36" s="158"/>
+    </row>
+    <row r="37" spans="1:31" s="4" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="B37" s="114">
         <v>8.1</v>
       </c>
-      <c r="C37" s="122" t="s">
-        <v>77</v>
-      </c>
-      <c r="D37" s="43"/>
-      <c r="E37" s="44"/>
-      <c r="F37" s="45"/>
-      <c r="G37" s="45"/>
-      <c r="H37" s="45"/>
-      <c r="I37" s="46"/>
-      <c r="J37" s="44"/>
-      <c r="K37" s="160"/>
-      <c r="L37" s="45"/>
-      <c r="M37" s="45"/>
-      <c r="N37" s="45"/>
-      <c r="O37" s="45"/>
-      <c r="P37" s="46"/>
-      <c r="Q37" s="118"/>
-      <c r="R37" s="46"/>
-    </row>
-    <row r="38" spans="1:31" s="4" customFormat="1" x14ac:dyDescent="0.4">
-      <c r="B38" s="51">
+      <c r="C37" s="116" t="s">
+        <v>62</v>
+      </c>
+      <c r="D37" s="38"/>
+      <c r="E37" s="39"/>
+      <c r="F37" s="40"/>
+      <c r="G37" s="40"/>
+      <c r="H37" s="40"/>
+      <c r="I37" s="41"/>
+      <c r="J37" s="39"/>
+      <c r="K37" s="148"/>
+      <c r="L37" s="40"/>
+      <c r="M37" s="40"/>
+      <c r="N37" s="40"/>
+      <c r="O37" s="40"/>
+      <c r="P37" s="41"/>
+      <c r="Q37" s="112"/>
+      <c r="R37" s="41"/>
+    </row>
+    <row r="38" spans="1:31" s="4" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="B38" s="46">
         <v>8.1999999999999993</v>
       </c>
-      <c r="C38" s="83" t="s">
-        <v>78</v>
-      </c>
-      <c r="D38" s="60"/>
-      <c r="E38" s="54"/>
-      <c r="F38" s="55"/>
-      <c r="G38" s="55"/>
-      <c r="H38" s="55"/>
-      <c r="I38" s="56"/>
-      <c r="J38" s="54"/>
-      <c r="K38" s="161"/>
-      <c r="L38" s="55"/>
-      <c r="M38" s="55"/>
-      <c r="N38" s="55"/>
-      <c r="O38" s="55"/>
-      <c r="P38" s="56"/>
-      <c r="Q38" s="57"/>
-      <c r="R38" s="56"/>
-    </row>
-    <row r="39" spans="1:31" s="4" customFormat="1" x14ac:dyDescent="0.4">
-      <c r="B39" s="81">
+      <c r="C38" s="77" t="s">
+        <v>63</v>
+      </c>
+      <c r="D38" s="54"/>
+      <c r="E38" s="48"/>
+      <c r="F38" s="49"/>
+      <c r="G38" s="49"/>
+      <c r="H38" s="49"/>
+      <c r="I38" s="50"/>
+      <c r="J38" s="48"/>
+      <c r="K38" s="149"/>
+      <c r="L38" s="49"/>
+      <c r="M38" s="49"/>
+      <c r="N38" s="49"/>
+      <c r="O38" s="49"/>
+      <c r="P38" s="50"/>
+      <c r="Q38" s="51"/>
+      <c r="R38" s="50"/>
+    </row>
+    <row r="39" spans="1:31" s="4" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="B39" s="75">
         <v>8.3000000000000007</v>
       </c>
-      <c r="C39" s="83" t="s">
-        <v>79</v>
-      </c>
-      <c r="D39" s="60"/>
-      <c r="E39" s="54"/>
-      <c r="F39" s="55"/>
-      <c r="G39" s="55"/>
-      <c r="H39" s="55"/>
-      <c r="I39" s="56"/>
-      <c r="J39" s="54"/>
-      <c r="K39" s="161"/>
-      <c r="L39" s="55"/>
-      <c r="M39" s="55"/>
-      <c r="N39" s="55"/>
-      <c r="O39" s="55"/>
-      <c r="P39" s="56"/>
-      <c r="Q39" s="57"/>
-      <c r="R39" s="56"/>
-    </row>
-    <row r="40" spans="1:31" s="4" customFormat="1" ht="15" thickBot="1" x14ac:dyDescent="0.45">
-      <c r="B40" s="74">
+      <c r="C39" s="77" t="s">
+        <v>64</v>
+      </c>
+      <c r="D39" s="54"/>
+      <c r="E39" s="48"/>
+      <c r="F39" s="49"/>
+      <c r="G39" s="49"/>
+      <c r="H39" s="49"/>
+      <c r="I39" s="50"/>
+      <c r="J39" s="48"/>
+      <c r="K39" s="149"/>
+      <c r="L39" s="49"/>
+      <c r="M39" s="49"/>
+      <c r="N39" s="49"/>
+      <c r="O39" s="49"/>
+      <c r="P39" s="50"/>
+      <c r="Q39" s="51"/>
+      <c r="R39" s="50"/>
+    </row>
+    <row r="40" spans="1:31" s="4" customFormat="1" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="B40" s="68">
         <v>8.4</v>
       </c>
-      <c r="C40" s="123" t="s">
-        <v>80</v>
-      </c>
-      <c r="D40" s="124"/>
-      <c r="E40" s="65"/>
-      <c r="F40" s="66"/>
-      <c r="G40" s="66"/>
-      <c r="H40" s="66"/>
-      <c r="I40" s="75"/>
-      <c r="J40" s="65"/>
-      <c r="K40" s="163"/>
-      <c r="L40" s="66"/>
-      <c r="M40" s="66"/>
-      <c r="N40" s="66"/>
-      <c r="O40" s="66"/>
-      <c r="P40" s="75"/>
-      <c r="Q40" s="76"/>
-      <c r="R40" s="75"/>
-    </row>
-    <row r="41" spans="1:31" ht="15" thickBot="1" x14ac:dyDescent="0.45">
-      <c r="B41" s="110">
+      <c r="C40" s="117" t="s">
+        <v>65</v>
+      </c>
+      <c r="D40" s="118"/>
+      <c r="E40" s="59"/>
+      <c r="F40" s="60"/>
+      <c r="G40" s="60"/>
+      <c r="H40" s="60"/>
+      <c r="I40" s="69"/>
+      <c r="J40" s="59"/>
+      <c r="K40" s="151"/>
+      <c r="L40" s="60"/>
+      <c r="M40" s="60"/>
+      <c r="N40" s="60"/>
+      <c r="O40" s="60"/>
+      <c r="P40" s="69"/>
+      <c r="Q40" s="70"/>
+      <c r="R40" s="69"/>
+    </row>
+    <row r="41" spans="1:31" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="B41" s="104">
         <v>9</v>
       </c>
-      <c r="C41" s="111" t="s">
-        <v>81</v>
-      </c>
-      <c r="D41" s="132"/>
-      <c r="E41" s="133"/>
-      <c r="F41" s="133"/>
-      <c r="G41" s="133"/>
-      <c r="H41" s="133"/>
-      <c r="I41" s="133"/>
-      <c r="J41" s="133"/>
-      <c r="K41" s="133"/>
-      <c r="L41" s="133"/>
-      <c r="M41" s="133"/>
-      <c r="N41" s="133"/>
-      <c r="O41" s="133"/>
-      <c r="P41" s="133"/>
-      <c r="Q41" s="133"/>
-      <c r="R41" s="134"/>
-    </row>
-    <row r="42" spans="1:31" s="2" customFormat="1" x14ac:dyDescent="0.4">
-      <c r="B42" s="41">
+      <c r="C41" s="105" t="s">
+        <v>66</v>
+      </c>
+      <c r="D41" s="156"/>
+      <c r="E41" s="157"/>
+      <c r="F41" s="157"/>
+      <c r="G41" s="157"/>
+      <c r="H41" s="157"/>
+      <c r="I41" s="157"/>
+      <c r="J41" s="157"/>
+      <c r="K41" s="157"/>
+      <c r="L41" s="157"/>
+      <c r="M41" s="157"/>
+      <c r="N41" s="157"/>
+      <c r="O41" s="157"/>
+      <c r="P41" s="157"/>
+      <c r="Q41" s="157"/>
+      <c r="R41" s="158"/>
+    </row>
+    <row r="42" spans="1:31" s="2" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="B42" s="36">
         <v>9.1</v>
       </c>
-      <c r="C42" s="125" t="s">
-        <v>87</v>
-      </c>
-      <c r="D42" s="126"/>
-      <c r="E42" s="127"/>
-      <c r="F42" s="128"/>
-      <c r="G42" s="128"/>
-      <c r="H42" s="128"/>
-      <c r="I42" s="129"/>
-      <c r="J42" s="130"/>
-      <c r="K42" s="160"/>
-      <c r="L42" s="48"/>
-      <c r="M42" s="48"/>
-      <c r="N42" s="48"/>
-      <c r="O42" s="48"/>
-      <c r="P42" s="49"/>
-      <c r="Q42" s="131"/>
-      <c r="R42" s="49"/>
-    </row>
-    <row r="43" spans="1:31" s="2" customFormat="1" x14ac:dyDescent="0.4">
-      <c r="B43" s="81">
+      <c r="C42" s="119" t="s">
+        <v>72</v>
+      </c>
+      <c r="D42" s="120"/>
+      <c r="E42" s="121"/>
+      <c r="F42" s="122"/>
+      <c r="G42" s="122"/>
+      <c r="H42" s="122"/>
+      <c r="I42" s="123"/>
+      <c r="J42" s="124"/>
+      <c r="K42" s="148"/>
+      <c r="L42" s="43"/>
+      <c r="M42" s="43"/>
+      <c r="N42" s="43"/>
+      <c r="O42" s="43"/>
+      <c r="P42" s="44"/>
+      <c r="Q42" s="125"/>
+      <c r="R42" s="44"/>
+    </row>
+    <row r="43" spans="1:31" s="2" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="B43" s="75">
         <v>9.1999999999999993</v>
       </c>
-      <c r="C43" s="84" t="s">
-        <v>84</v>
-      </c>
-      <c r="D43" s="85"/>
-      <c r="E43" s="86"/>
-      <c r="F43" s="87"/>
-      <c r="G43" s="62"/>
-      <c r="H43" s="62"/>
-      <c r="I43" s="58"/>
-      <c r="J43" s="91"/>
-      <c r="K43" s="161"/>
-      <c r="L43" s="62"/>
-      <c r="M43" s="62"/>
-      <c r="N43" s="62"/>
-      <c r="O43" s="62"/>
-      <c r="P43" s="58"/>
-      <c r="Q43" s="90"/>
-      <c r="R43" s="58"/>
-    </row>
-    <row r="44" spans="1:31" s="2" customFormat="1" x14ac:dyDescent="0.4">
-      <c r="B44" s="51">
+      <c r="C43" s="78" t="s">
+        <v>69</v>
+      </c>
+      <c r="D43" s="79"/>
+      <c r="E43" s="80"/>
+      <c r="F43" s="81"/>
+      <c r="G43" s="56"/>
+      <c r="H43" s="56"/>
+      <c r="I43" s="52"/>
+      <c r="J43" s="85"/>
+      <c r="K43" s="149"/>
+      <c r="L43" s="56"/>
+      <c r="M43" s="56"/>
+      <c r="N43" s="56"/>
+      <c r="O43" s="56"/>
+      <c r="P43" s="52"/>
+      <c r="Q43" s="84"/>
+      <c r="R43" s="52"/>
+    </row>
+    <row r="44" spans="1:31" s="2" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="B44" s="46">
         <v>9.3000000000000007</v>
       </c>
-      <c r="C44" s="84" t="s">
-        <v>85</v>
-      </c>
-      <c r="D44" s="53"/>
-      <c r="E44" s="61"/>
-      <c r="F44" s="62"/>
-      <c r="G44" s="62"/>
-      <c r="H44" s="62"/>
-      <c r="I44" s="88"/>
-      <c r="J44" s="89"/>
-      <c r="K44" s="161"/>
-      <c r="L44" s="87"/>
-      <c r="M44" s="62"/>
-      <c r="N44" s="62"/>
-      <c r="O44" s="62"/>
-      <c r="P44" s="92"/>
-      <c r="Q44" s="90"/>
-      <c r="R44" s="58"/>
-    </row>
-    <row r="45" spans="1:31" s="2" customFormat="1" x14ac:dyDescent="0.4">
-      <c r="B45" s="81">
+      <c r="C44" s="78" t="s">
+        <v>70</v>
+      </c>
+      <c r="D44" s="47"/>
+      <c r="E44" s="55"/>
+      <c r="F44" s="56"/>
+      <c r="G44" s="82"/>
+      <c r="H44" s="82"/>
+      <c r="I44" s="82"/>
+      <c r="J44" s="83"/>
+      <c r="K44" s="149"/>
+      <c r="L44" s="81"/>
+      <c r="M44" s="56"/>
+      <c r="N44" s="56"/>
+      <c r="O44" s="56"/>
+      <c r="P44" s="86"/>
+      <c r="Q44" s="84"/>
+      <c r="R44" s="52"/>
+    </row>
+    <row r="45" spans="1:31" s="2" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="B45" s="75">
         <v>9.4</v>
       </c>
-      <c r="C45" s="84" t="s">
-        <v>86</v>
-      </c>
-      <c r="D45" s="53"/>
-      <c r="E45" s="61"/>
-      <c r="F45" s="62"/>
-      <c r="G45" s="62"/>
-      <c r="H45" s="62"/>
-      <c r="I45" s="88"/>
-      <c r="J45" s="89"/>
-      <c r="K45" s="161"/>
-      <c r="L45" s="62"/>
-      <c r="M45" s="62"/>
-      <c r="N45" s="62"/>
-      <c r="O45" s="62"/>
-      <c r="P45" s="88"/>
-      <c r="Q45" s="93"/>
-      <c r="R45" s="58"/>
-    </row>
-    <row r="46" spans="1:31" ht="15" thickBot="1" x14ac:dyDescent="0.45">
-      <c r="B46" s="73">
+      <c r="C45" s="78" t="s">
+        <v>71</v>
+      </c>
+      <c r="D45" s="47"/>
+      <c r="E45" s="55"/>
+      <c r="F45" s="56"/>
+      <c r="G45" s="56"/>
+      <c r="H45" s="56"/>
+      <c r="I45" s="82"/>
+      <c r="J45" s="83"/>
+      <c r="K45" s="149"/>
+      <c r="L45" s="56"/>
+      <c r="M45" s="56"/>
+      <c r="N45" s="56"/>
+      <c r="O45" s="56"/>
+      <c r="P45" s="82"/>
+      <c r="Q45" s="87"/>
+      <c r="R45" s="52"/>
+    </row>
+    <row r="46" spans="1:31" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="B46" s="67">
         <v>9.5</v>
       </c>
-      <c r="C46" s="94" t="s">
-        <v>88</v>
-      </c>
-      <c r="D46" s="95"/>
-      <c r="E46" s="96"/>
-      <c r="F46" s="97"/>
-      <c r="G46" s="97"/>
-      <c r="H46" s="97"/>
-      <c r="I46" s="98"/>
-      <c r="J46" s="96"/>
-      <c r="K46" s="162"/>
-      <c r="L46" s="97"/>
-      <c r="M46" s="97"/>
-      <c r="N46" s="97"/>
-      <c r="O46" s="97"/>
-      <c r="P46" s="98"/>
-      <c r="Q46" s="99"/>
-      <c r="R46" s="98"/>
-    </row>
-    <row r="50" spans="3:6" x14ac:dyDescent="0.4">
+      <c r="C46" s="88" t="s">
+        <v>73</v>
+      </c>
+      <c r="D46" s="89"/>
+      <c r="E46" s="90"/>
+      <c r="F46" s="91"/>
+      <c r="G46" s="91"/>
+      <c r="H46" s="91"/>
+      <c r="I46" s="92"/>
+      <c r="J46" s="90"/>
+      <c r="K46" s="150"/>
+      <c r="L46" s="91"/>
+      <c r="M46" s="91"/>
+      <c r="N46" s="91"/>
+      <c r="O46" s="91"/>
+      <c r="P46" s="92"/>
+      <c r="Q46" s="93"/>
+      <c r="R46" s="92"/>
+    </row>
+    <row r="50" spans="3:6" x14ac:dyDescent="0.25">
       <c r="C50" s="3" t="s">
+        <v>50</v>
+      </c>
+      <c r="D50" s="3" t="s">
+        <v>67</v>
+      </c>
+    </row>
+    <row r="51" spans="3:6" x14ac:dyDescent="0.25">
+      <c r="C51" s="5" t="s">
+        <v>51</v>
+      </c>
+      <c r="D51" s="159" t="s">
+        <v>16</v>
+      </c>
+      <c r="E51" s="159"/>
+      <c r="F51" s="159"/>
+    </row>
+    <row r="52" spans="3:6" x14ac:dyDescent="0.25">
+      <c r="C52" s="5" t="s">
         <v>52</v>
       </c>
-      <c r="D50" s="3" t="s">
-        <v>82</v>
-      </c>
-    </row>
-    <row r="51" spans="3:6" x14ac:dyDescent="0.4">
-      <c r="C51" s="5" t="s">
+      <c r="D52" s="160" t="s">
+        <v>31</v>
+      </c>
+      <c r="E52" s="160"/>
+      <c r="F52" s="160"/>
+    </row>
+    <row r="53" spans="3:6" x14ac:dyDescent="0.25">
+      <c r="C53" s="5" t="s">
+        <v>53</v>
+      </c>
+      <c r="D53" s="161" t="s">
+        <v>39</v>
+      </c>
+      <c r="E53" s="161"/>
+      <c r="F53" s="161"/>
+    </row>
+    <row r="54" spans="3:6" x14ac:dyDescent="0.25">
+      <c r="C54" s="5" t="s">
         <v>54</v>
       </c>
-      <c r="D51" s="37" t="s">
-        <v>16</v>
-      </c>
-      <c r="E51" s="37"/>
-      <c r="F51" s="37"/>
-    </row>
-    <row r="52" spans="3:6" x14ac:dyDescent="0.4">
-      <c r="C52" s="5" t="s">
+      <c r="D54" s="162" t="s">
+        <v>43</v>
+      </c>
+      <c r="E54" s="162"/>
+      <c r="F54" s="162"/>
+    </row>
+    <row r="55" spans="3:6" x14ac:dyDescent="0.25">
+      <c r="C55" s="5" t="s">
+        <v>55</v>
+      </c>
+      <c r="D55" s="163" t="s">
+        <v>47</v>
+      </c>
+      <c r="E55" s="164"/>
+      <c r="F55" s="165"/>
+    </row>
+    <row r="56" spans="3:6" x14ac:dyDescent="0.25">
+      <c r="C56" s="5" t="s">
         <v>56</v>
-      </c>
-      <c r="D52" s="38" t="s">
-        <v>31</v>
-      </c>
-      <c r="E52" s="38"/>
-      <c r="F52" s="38"/>
-    </row>
-    <row r="53" spans="3:6" x14ac:dyDescent="0.4">
-      <c r="C53" s="5" t="s">
-        <v>58</v>
-      </c>
-      <c r="D53" s="39" t="s">
-        <v>39</v>
-      </c>
-      <c r="E53" s="39"/>
-      <c r="F53" s="39"/>
-    </row>
-    <row r="54" spans="3:6" x14ac:dyDescent="0.4">
-      <c r="C54" s="5" t="s">
-        <v>60</v>
-      </c>
-      <c r="D54" s="40" t="s">
-        <v>44</v>
-      </c>
-      <c r="E54" s="40"/>
-      <c r="F54" s="40"/>
-    </row>
-    <row r="55" spans="3:6" x14ac:dyDescent="0.4">
-      <c r="C55" s="5" t="s">
-        <v>62</v>
-      </c>
-      <c r="D55" s="165" t="s">
-        <v>48</v>
-      </c>
-      <c r="E55" s="166"/>
-      <c r="F55" s="167"/>
-    </row>
-    <row r="56" spans="3:6" x14ac:dyDescent="0.4">
-      <c r="C56" s="5" t="s">
-        <v>64</v>
       </c>
     </row>
   </sheetData>
   <mergeCells count="14">
+    <mergeCell ref="D55:F55"/>
+    <mergeCell ref="D11:R11"/>
+    <mergeCell ref="D14:R14"/>
+    <mergeCell ref="D41:R41"/>
+    <mergeCell ref="D36:R36"/>
+    <mergeCell ref="D51:F51"/>
+    <mergeCell ref="D52:F52"/>
+    <mergeCell ref="D53:F53"/>
+    <mergeCell ref="D54:F54"/>
     <mergeCell ref="D7:R7"/>
     <mergeCell ref="D17:R17"/>
     <mergeCell ref="D24:R24"/>
     <mergeCell ref="D32:R32"/>
     <mergeCell ref="D34:R34"/>
-    <mergeCell ref="D36:R36"/>
-    <mergeCell ref="D51:F51"/>
-    <mergeCell ref="D52:F52"/>
-    <mergeCell ref="D53:F53"/>
-    <mergeCell ref="D54:F54"/>
-    <mergeCell ref="D55:F55"/>
-    <mergeCell ref="D11:R11"/>
-    <mergeCell ref="D14:R14"/>
-    <mergeCell ref="D41:R41"/>
   </mergeCells>
   <pageMargins left="0.70078740157480324" right="0.70078740157480324" top="0.75196850393700787" bottom="0.75196850393700787" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" firstPageNumber="2147483648" orientation="portrait"/>
+  <drawing r:id="rId1"/>
 </worksheet>
 </file>
</xml_diff>